<commit_message>
Pasta DiagramaS de sequencias
</commit_message>
<xml_diff>
--- a/Cronogramas/Cronogramas.xlsx
+++ b/Cronogramas/Cronogramas.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\Documents\DACSistemaRH\Cronogramas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma Telas" sheetId="1" r:id="rId1"/>
@@ -181,7 +176,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -583,7 +578,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1071,7 +1066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1083,7 +1078,7 @@
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1504,8 +1499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Casos de uso (parcial)
</commit_message>
<xml_diff>
--- a/Cronogramas/Cronogramas.xlsx
+++ b/Cronogramas/Cronogramas.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mths\Desktop\Projeto DAC\DACSistemaRH\Cronogramas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma Telas" sheetId="1" r:id="rId1"/>
     <sheet name="Cronograma Casos de Uso" sheetId="2" r:id="rId2"/>
     <sheet name="Cronograma Diagrama Sequencia" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -239,13 +244,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,7 +584,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1066,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I8" activeCellId="1" sqref="I9 I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,9 +1137,9 @@
       <c r="G2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="3"/>
+      <c r="H2" s="5"/>
       <c r="I2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1282,7 +1288,7 @@
         <v>43043</v>
       </c>
       <c r="H8" s="5"/>
-      <c r="I8" t="s">
+      <c r="I8" s="6" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1306,9 +1312,9 @@
       <c r="G9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" t="s">
-        <v>49</v>
+      <c r="H9" s="5"/>
+      <c r="I9" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1499,7 +1505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Clovis daniel gueno 25/04/2017
</commit_message>
<xml_diff>
--- a/Cronogramas/Cronogramas.xlsx
+++ b/Cronogramas/Cronogramas.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
@@ -11,12 +11,7 @@
     <sheet name="Cronograma Casos de Uso" sheetId="2" r:id="rId2"/>
     <sheet name="Cronograma Diagrama Sequencia" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -177,7 +172,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +191,13 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -239,13 +241,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -255,9 +258,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -578,7 +578,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1067,7 +1067,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,7 +1500,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I10" sqref="I10:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1713,9 +1713,9 @@
       <c r="G8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="3"/>
+      <c r="H8" s="6"/>
       <c r="I8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1763,9 +1763,9 @@
       <c r="G10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="3"/>
+      <c r="H10" s="6"/>
       <c r="I10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1788,9 +1788,9 @@
       <c r="G11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="3"/>
+      <c r="H11" s="6"/>
       <c r="I11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1813,9 +1813,9 @@
       <c r="G12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="3"/>
+      <c r="H12" s="6"/>
       <c r="I12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1920,8 +1920,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>